<commit_message>
Fixed Mailchimp Mailing List Integration
</commit_message>
<xml_diff>
--- a/yurs2016/Finalists.xlsx
+++ b/yurs2016/Finalists.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\surya\Dropbox\Yale\Extracurriculars\YURA\YURS\2016\Applications\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\surya\Dropbox\Yale\Extracurriculars\YURA\Website\YURAresearch.github.io\yurs2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -467,10 +467,6 @@
 </t>
   </si>
   <si>
-    <t>Gun violence remains a pervasive problem in the United States. While shootings are seemingly random, a growing body of literature suggests that patterns of gun violence share striking similarities with the transmission patterns of other public health epidemics, such as HIV/AIDS and obesity. In particular, recent research has hypothesized that exposure to victims of gun violence in an individualâ€™s co-offending network significantly affects the individualâ€™s likelihood of victimization. While this theory has been confirmed in Boston and Chicago, more studies are needed to test its generalizability across various cities and communities.
-Our study contributes to the existing literature by assessing the spread of gun violence in seven American cities: Cincinnati, East Palo Alto, Hartford, Newark, New Orleans, Oakland, and Stockton. Specifically, we investigated the extent to which oneâ€™s likelihood of victimization is associated with direct and indirect exposure to gun violence victims in co-offending networks. Using police data on gunshot victimization and co-arrests, we reconstructed patterns of co-offending and located gunshot victims within the network for each city. We ran a series of logistic regression models with victimization status (1 = yes, 0 = no) as the independent variable and individual risk factors, including gender, gang membership, age, degree, race, and exposure to victims in oneâ€™s social network, as dependent variables. The results from regression analysis show that the probability of victimization is strongly associated with the level of network exposure to gunshot victims in six out of the seven cities. While preliminary, these results predominantly support the theory that the distribution of gun victimization in co-offending networks follows a pattern indicative of social contagion. Such pattern of gun violence in social networks has important implications for understanding Americaâ€™s gun violence epidemic and for developing effective policies to curb it.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Non-scalpel vasectomy is a procedure for male permanent sterilization that is safer, more effective, and painless compared to other forms of male or female sterilization. Despite extensive efforts on behalf of Indian governmental programs as well as individual hospitals and clinics, the uptake of non-scalpel vasectomy in Pune, Maharashtra remains very low. This study investigated local communityâ€™s perceptions of non-scalpel vasectomy with the goal of utilizing this information to increase uptake. Research took place at the Family Planning Association of Pune on Ganeshkind Road. Using a semi-structured questionnaire, 50 patients of the FPA were interviewed, half men and half women. Each interview collected a standard set of demographics, information regarding the culture of family planning decisions, and opinions of NSV. It was hypothesized that most subjects would initially be unfamiliar with NSV. Even after a professional explanation that was aimed to dispel misconceptions, it was expected to find that patients would still be resistant to the procedure due to fears regarding the operation and negative influence from the community. After field research, quantitative and qualitative data was analyzed and discussed to determine means and trends. A slight majority of the subject pool had knowledge of NSV. Most subjects answered that family planning was the coupleâ€™s decision, however, qualitative data revealed that tubectomy was usually chosen instead due to the belief that family planning is the womanâ€™s responsibility. The highest reported fear was of community judgments, followed by impact to masculinity, and then concern of pain. It is recommended that information of NSV continues to be disseminated through hospitals, clinics, and media to provide correct information. Advocacy by patients who have accepted NSV would help destigmatize the procedure. These results will help governmental programs, hospitals, and clinics understand the necessary interventions in order to dispel misconceptions of NSV and increase uptake.
 </t>
   </si>
@@ -653,6 +649,9 @@
   </si>
   <si>
     <t>Will Bring Own (56"x36")</t>
+  </si>
+  <si>
+    <t>Gun violence remains a pervasive problem in the United States. In 2013 alone, 11,208 individuals were murdered and approximately 62,220 others were injured with firearms. While seemingly random, a growing body of literature suggests that the contagion patterns of gun violence share striking similarities with the transmission patterns of other public health epidemics, such as HIV/AIDS and obesity. In particular, recent research has hypothesized that exposure to victims of gun violence in an individual’s co-offending network significantly affects the individual’s likelihood of victimization. While this theory has been confirmed in Boston and Chicago, more studies are needed to test its generalizability across cities and communities. Our study contributes to the existing literature by assessing the contagion pattern of gun violence in seven American cities. We investigated the extent to which one’s likelihood of victimization is associated with direct and indirect exposure to gun violence victims in co-offending networks. Using police data, we reconstructed patterns of co-offending and located gunshot victims within the network for each city. We ran a series of logistic regression models with victimization status as the dependent variable and individual risk factors, including gender, gang membership, age, degree, race, and exposure to victims in one’s social network, as independent variables. The results from regression analysis show that the probability of victimization is strongly associated with the level of network exposure to gunshot victims in six out of the seven cities. These results predominantly support the theory that the distribution of gun victimization in co-offending networks follows a pattern indicative of social contagion. Such pattern of gun violence in social networks has important implications for understanding America’s gun violence epidemic and developing effective public health policies to curb it.</t>
   </si>
 </sst>
 </file>
@@ -1211,120 +1210,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Year" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A20:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="1">
-    <pivotField axis="axisRow" dataField="1" showAll="0">
-      <items count="10">
-        <item x="5"/>
-        <item x="7"/>
-        <item x="4"/>
-        <item x="8"/>
-        <item x="6"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="10">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Fields" fld="0" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A7:B18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
@@ -1387,6 +1272,120 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Count of College" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:B5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Year" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A20:B30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
+    <pivotField axis="axisRow" dataField="1" showAll="0">
+      <items count="10">
+        <item x="5"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Fields" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1662,9 +1661,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1691,7 +1690,7 @@
         <v>121</v>
       </c>
       <c r="D1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E1" t="s">
         <v>122</v>
@@ -1706,7 +1705,7 @@
         <v>125</v>
       </c>
       <c r="I1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1720,7 +1719,7 @@
         <v>75</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E2">
         <v>2018</v>
@@ -1729,13 +1728,13 @@
         <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H2" t="s">
         <v>76</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J2" s="1"/>
     </row>
@@ -1750,7 +1749,7 @@
         <v>57</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3">
         <v>2018</v>
@@ -1759,13 +1758,13 @@
         <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -1780,7 +1779,7 @@
         <v>97</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E4">
         <v>2017</v>
@@ -1789,10 +1788,10 @@
         <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>136</v>
@@ -1810,7 +1809,7 @@
         <v>17</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5">
         <v>2018</v>
@@ -1840,7 +1839,7 @@
         <v>61</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E6">
         <v>2018</v>
@@ -1849,13 +1848,13 @@
         <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -1870,7 +1869,7 @@
         <v>53</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7">
         <v>2018</v>
@@ -1879,13 +1878,13 @@
         <v>54</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H7" t="s">
         <v>55</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J7" s="1"/>
     </row>
@@ -1900,7 +1899,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E8">
         <v>2019</v>
@@ -1909,7 +1908,7 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H8" t="s">
         <v>33</v>
@@ -1930,7 +1929,7 @@
         <v>63</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E9">
         <v>2019</v>
@@ -1939,13 +1938,13 @@
         <v>2</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -1960,7 +1959,7 @@
         <v>72</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E10">
         <v>2017</v>
@@ -1969,13 +1968,13 @@
         <v>28</v>
       </c>
       <c r="G10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H10" t="s">
         <v>73</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1989,7 +1988,7 @@
         <v>48</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E11">
         <v>2017</v>
@@ -1998,13 +1997,13 @@
         <v>49</v>
       </c>
       <c r="G11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H11" t="s">
         <v>51</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>139</v>
+        <v>194</v>
       </c>
       <c r="J11" s="1"/>
     </row>
@@ -2019,7 +2018,7 @@
         <v>69</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E12">
         <v>2019</v>
@@ -2028,13 +2027,13 @@
         <v>14</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H12" t="s">
         <v>70</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J12" s="1"/>
     </row>
@@ -2049,7 +2048,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E13">
         <v>2017</v>
@@ -2079,7 +2078,7 @@
         <v>65</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E14">
         <v>2019</v>
@@ -2088,13 +2087,13 @@
         <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H14" t="s">
         <v>67</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J14" s="1"/>
     </row>
@@ -2109,7 +2108,7 @@
         <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E15">
         <v>2018</v>
@@ -2118,7 +2117,7 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H15" t="s">
         <v>39</v>
@@ -2139,7 +2138,7 @@
         <v>102</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E16">
         <v>2017</v>
@@ -2148,13 +2147,13 @@
         <v>28</v>
       </c>
       <c r="G16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J16" s="1"/>
     </row>
@@ -2169,7 +2168,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E17">
         <v>2017</v>
@@ -2199,7 +2198,7 @@
         <v>59</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E18">
         <v>2019</v>
@@ -2208,13 +2207,13 @@
         <v>54</v>
       </c>
       <c r="G18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J18" s="1"/>
     </row>
@@ -2229,7 +2228,7 @@
         <v>82</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E19">
         <v>2018</v>
@@ -2238,13 +2237,13 @@
         <v>83</v>
       </c>
       <c r="G19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H19" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2258,7 +2257,7 @@
         <v>46</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E20">
         <v>2019</v>
@@ -2267,10 +2266,10 @@
         <v>2</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>138</v>
@@ -2288,7 +2287,7 @@
         <v>24</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E21">
         <v>2017</v>
@@ -2300,7 +2299,7 @@
         <v>126</v>
       </c>
       <c r="H21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>134</v>
@@ -2318,7 +2317,7 @@
         <v>91</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E22">
         <v>2017</v>
@@ -2330,7 +2329,7 @@
         <v>126</v>
       </c>
       <c r="H22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I22" t="s">
         <v>131</v>
@@ -2348,7 +2347,7 @@
         <v>20</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E23">
         <v>2017</v>
@@ -2378,7 +2377,7 @@
         <v>78</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E24">
         <v>2017</v>
@@ -2387,13 +2386,13 @@
         <v>79</v>
       </c>
       <c r="G24" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H24" t="s">
         <v>80</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J24" s="1"/>
     </row>
@@ -2408,7 +2407,7 @@
         <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E25">
         <v>2017</v>
@@ -2417,13 +2416,13 @@
         <v>28</v>
       </c>
       <c r="G25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H25" t="s">
         <v>29</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J25" s="1"/>
     </row>
@@ -2438,7 +2437,7 @@
         <v>6</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E26">
         <v>2018</v>
@@ -2468,7 +2467,7 @@
         <v>117</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E27">
         <v>2017</v>
@@ -2477,13 +2476,13 @@
         <v>25</v>
       </c>
       <c r="G27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H27" t="s">
         <v>118</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J27" s="1"/>
     </row>
@@ -2585,10 +2584,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2617,7 +2616,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" s="4">
         <v>26</v>
@@ -2625,10 +2624,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2713,7 +2712,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B18" s="4">
         <v>26</v>
@@ -2721,15 +2720,15 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B21" s="4">
         <v>2</v>
@@ -2737,7 +2736,7 @@
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B22" s="4">
         <v>3</v>
@@ -2745,7 +2744,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B23" s="4">
         <v>3</v>
@@ -2753,7 +2752,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
@@ -2761,7 +2760,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B25" s="4">
         <v>2</v>
@@ -2769,7 +2768,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B26" s="4">
         <v>8</v>
@@ -2777,7 +2776,7 @@
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B27" s="4">
         <v>5</v>
@@ -2793,7 +2792,7 @@
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" s="4">
         <v>5</v>
@@ -2801,7 +2800,7 @@
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B30" s="4">
         <v>44</v>

</xml_diff>